<commit_message>
implemented a new list in documentation_gui-module and a method to fill this list, aggregating information of relevant material isn't implemented yet
</commit_message>
<xml_diff>
--- a/data/SUN 24-001/articles.xlsx
+++ b/data/SUN 24-001/articles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3441\Documents\Familie\Edgar\Weiterbildungen\Kurse\Python Bootcamp\Projekte\SUN-Artikel-Fetcher\db\SUN 24-001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3441\Documents\Familie\Edgar\Weiterbildungen\Kurse\Python Bootcamp\Projekte\SUN_Article_Fetcher\data\SUN 24-001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17F72BC7-7D5F-437A-918B-E5B4ED3D9F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F7D3A8-33B5-49F0-A042-07D102CF828B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="930" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="articles" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>000001</t>
   </si>
@@ -62,12 +62,27 @@
   </si>
   <si>
     <t>Material 100</t>
+  </si>
+  <si>
+    <t>AC-Kopplung</t>
+  </si>
+  <si>
+    <t>Batteriemodul</t>
+  </si>
+  <si>
+    <t>BCU</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>BWR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -607,9 +622,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -647,7 +662,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -753,7 +768,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -895,116 +910,176 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>4635687678</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>4564596899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4564596899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4564596899</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GUI-documentation-module: added buttons to each table for removing articles from list; Functions: added ability of removing articles from each table add putting them onto to the related section in blacklist; changed the functions of interest into a state in which they can be used in relation to the selected table
</commit_message>
<xml_diff>
--- a/data/SUN 24-001/articles.xlsx
+++ b/data/SUN 24-001/articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3441\Documents\Familie\Edgar\Weiterbildungen\Kurse\Python Bootcamp\Projekte\SUN_Article_Fetcher\data\SUN 24-001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F7D3A8-33B5-49F0-A042-07D102CF828B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9562AD-6F93-4106-916D-546EEB8A2B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>000001</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>BWR</t>
+  </si>
+  <si>
+    <t>000011</t>
+  </si>
+  <si>
+    <t>000012</t>
+  </si>
+  <si>
+    <t>000203</t>
   </si>
 </sst>
 </file>
@@ -921,7 +930,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1027,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1029,7 +1038,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -1040,7 +1049,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -1051,7 +1060,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
started implementing data_handling of device specs by storing manually typed data to into cells of device lists, not done yet
</commit_message>
<xml_diff>
--- a/data/SUN 24-001/articles.xlsx
+++ b/data/SUN 24-001/articles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3441\Documents\Familie\Edgar\Weiterbildungen\Kurse\Python Bootcamp\Projekte\SUN_Article_Fetcher\data\SUN 24-001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9562AD-6F93-4106-916D-546EEB8A2B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC83DE0-6D9A-4A91-AF9C-33C9593D2EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>000001</t>
   </si>
@@ -43,9 +43,6 @@
     <t>000004</t>
   </si>
   <si>
-    <t>Material 4</t>
-  </si>
-  <si>
     <t>000006</t>
   </si>
   <si>
@@ -86,13 +83,64 @@
   </si>
   <si>
     <t>000203</t>
+  </si>
+  <si>
+    <t>000005</t>
+  </si>
+  <si>
+    <t>WR 3</t>
+  </si>
+  <si>
+    <t>000067</t>
+  </si>
+  <si>
+    <t>000068</t>
+  </si>
+  <si>
+    <t>000069</t>
+  </si>
+  <si>
+    <t>000070</t>
+  </si>
+  <si>
+    <t>000071</t>
+  </si>
+  <si>
+    <t>000072</t>
+  </si>
+  <si>
+    <t>000073</t>
+  </si>
+  <si>
+    <t>000074</t>
+  </si>
+  <si>
+    <t>Modul-Typ_1</t>
+  </si>
+  <si>
+    <t>Ladestation Typ 1</t>
+  </si>
+  <si>
+    <t>Ladestation Typ 2</t>
+  </si>
+  <si>
+    <t>Material 71</t>
+  </si>
+  <si>
+    <t>Material 72</t>
+  </si>
+  <si>
+    <t>Material 73</t>
+  </si>
+  <si>
+    <t>Material 74</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +271,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -927,20 +981,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -948,11 +1006,8 @@
       <c r="D1">
         <v>4635687678</v>
       </c>
-      <c r="E1">
-        <v>5</v>
-      </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -960,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -974,7 +1029,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -988,7 +1043,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -996,19 +1051,16 @@
       <c r="D4">
         <v>4564596899</v>
       </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1016,10 +1068,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1027,7 +1079,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1038,7 +1090,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -1049,7 +1101,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -1060,7 +1112,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -1071,10 +1123,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1082,16 +1134,117 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>6788596899</v>
+      </c>
+      <c r="F13" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
-        <v>1</v>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>4357768878</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>8769868878</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20">
+        <v>354</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>